<commit_message>
Created finished script for loading data
</commit_message>
<xml_diff>
--- a/student-mat.xlsx
+++ b/student-mat.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frede\Documents\UNI\Baby Machines Learning\Student Performance Prediction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frede\Documents\UNI\Baby Machines Learning\Student Performance Prediction\2450Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC36A61-97A7-4F95-AE72-E890F7976721}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386EF05A-0541-4761-A07C-C2476B593123}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BC2807ED-F122-47E3-922C-9D1D69611561}"/>
   </bookViews>
@@ -421,7 +421,7 @@
   <dimension ref="A1:L396"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>